<commit_message>
Started tests for standard and custom games
</commit_message>
<xml_diff>
--- a/TCJPClueLayout.xlsx
+++ b/TCJPClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameTCJP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="30">
   <si>
     <t>w</t>
   </si>
@@ -96,13 +96,31 @@
   </si>
   <si>
     <t>RL</t>
+  </si>
+  <si>
+    <t>Door direction tests (TCJP_FileInitTests)</t>
+  </si>
+  <si>
+    <t>Walkway adjacency test</t>
+  </si>
+  <si>
+    <t>Internal room space test</t>
+  </si>
+  <si>
+    <t>Adjacency lists, room entrances</t>
+  </si>
+  <si>
+    <t>Adjacency lists, walkways to room entrances</t>
+  </si>
+  <si>
+    <t>Number of doors: 16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +128,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +167,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,18 +210,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF99"/>
+      <color rgb="FFCC00FF"/>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -441,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +522,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -462,7 +531,7 @@
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -495,7 +564,7 @@
       <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -692,7 +761,7 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -800,7 +869,7 @@
       <c r="L5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="4" t="s">
@@ -863,7 +932,7 @@
       <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="10" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -941,7 +1010,7 @@
       <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -998,7 +1067,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1013,7 +1082,7 @@
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1052,7 +1121,7 @@
       <c r="R8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="T8" s="3" t="s">
@@ -1457,7 +1526,7 @@
       <c r="W13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="X13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="Y13">
@@ -1613,7 +1682,7 @@
       <c r="W15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="X15" s="3" t="s">
+      <c r="X15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="Y15">
@@ -1784,7 +1853,7 @@
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1955,7 +2024,7 @@
       <c r="G20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2033,7 +2102,7 @@
       <c r="G21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="10" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -2042,10 +2111,10 @@
       <c r="J21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3" t="s">
+      <c r="K21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>15</v>
       </c>
       <c r="M21" s="4" t="s">
@@ -2210,7 +2279,7 @@
       <c r="N23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="P23" s="4" t="s">
@@ -2333,10 +2402,10 @@
       <c r="C25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2354,7 +2423,7 @@
       <c r="J25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="L25" s="4" t="s">
@@ -2496,6 +2565,41 @@
       <c r="X26">
         <f t="shared" si="1"/>
         <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests passed for move targeting
</commit_message>
<xml_diff>
--- a/TCJPClueLayout.xlsx
+++ b/TCJPClueLayout.xlsx
@@ -513,7 +513,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1586,7 @@
       <c r="Q14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="S14" s="1" t="s">

</xml_diff>